<commit_message>
fix: Add compute_spatial_entropy function to fix fig05 panel C
- Previously looked for pre-computed entropy in adata.obs
- Now computes Shannon entropy directly from cell type distributions
- Regenerated fig05 with actual spatial entropy values
- Updated data tables with computed entropy metrics

Spatial entropy findings:
- Responders: 3.70 (higher diversity)
- Non-Responders: 3.47 (lower diversity)
- Cohen's d = 5.06 (large effect, descriptive only)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tables/T4_spatial_metrics.xlsx
+++ b/tables/T4_spatial_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>spatial_entropy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>diversity_shannon</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>n_cell_types</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>tissue_area</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>mean_nn_dist</t>
         </is>
@@ -485,15 +490,18 @@
         <v>914</v>
       </c>
       <c r="D2" t="n">
+        <v>3.681212142935576</v>
+      </c>
+      <c r="E2" t="n">
         <v>2.551621816518829</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>14</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>40248263</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>109.4206014792818</v>
       </c>
     </row>
@@ -512,15 +520,18 @@
         <v>1407</v>
       </c>
       <c r="D3" t="n">
+        <v>3.720209773733151</v>
+      </c>
+      <c r="E3" t="n">
         <v>2.578652914354685</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>14</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>58881143.50000001</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>122.7127637852222</v>
       </c>
     </row>
@@ -539,15 +550,18 @@
         <v>863</v>
       </c>
       <c r="D4" t="n">
+        <v>3.508339164031677</v>
+      </c>
+      <c r="E4" t="n">
         <v>2.431795398596592</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>14</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>52312308</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>122.8278556344391</v>
       </c>
     </row>
@@ -566,15 +580,18 @@
         <v>1914</v>
       </c>
       <c r="D5" t="n">
+        <v>3.424244434780839</v>
+      </c>
+      <c r="E5" t="n">
         <v>2.373505374116422</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>14</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>46978009.50000001</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>107.614229631433</v>
       </c>
     </row>

</xml_diff>